<commit_message>
Attendance 10_08_2023 on 12:18AM
Attendance 10_08_2023 on 12:18AM
</commit_message>
<xml_diff>
--- a/React-B1-AttendanceManagement.xlsx
+++ b/React-B1-AttendanceManagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\attendanceMentainace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A5C139-CD67-450D-B161-859DFC6F7DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFC51E4-E449-49E5-8396-682ACADC12E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1115,12 +1115,132 @@
         </r>
       </text>
     </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{13FE914F-79F5-4DBA-8FB7-54FAEBDFF9AE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Office work</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{D1025057-79CD-4A4D-A366-D3C746A93C36}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Note Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{1E770157-4FA4-4664-8A79-C7CE90268FA4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Note Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P11" authorId="0" shapeId="0" xr:uid="{75CDE8A6-0385-4898-815F-451D11ED4EC8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Note Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q11" authorId="0" shapeId="0" xr:uid="{DDDEE947-57E3-4A13-8B70-1562EAD182BD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Note Responded</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -1743,7 +1863,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11:T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2390,22 +2510,63 @@
       <c r="A11" s="5">
         <v>45148</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" s="10">
+        <v>16</v>
+      </c>
+      <c r="S11" s="12">
+        <v>11</v>
+      </c>
+      <c r="T11" s="11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
@@ -17942,10 +18103,10 @@
   <dataConsolidate/>
   <dataValidations count="3">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{6155AC06-7F61-4A08-843D-AAA25B377341}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:G15 B11:B25 I18:P123 B5:P6 I124:K1048576 I2:P4 B2:G4 F22:G22 D23:G25 D18:G21 B26:G1048576 B8:H10 J11:P15 J8:P9 J10:K10 M10:P10" xr:uid="{26F8D555-BFDA-E840-969B-30EA98F09544}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B25 J11:P15 I18:P123 B5:P6 I124:K1048576 I2:P4 B2:G4 F22:G22 D23:G25 D18:G21 B26:G1048576 B8:H10 M10:P10 J8:P9 J10:K10 D12:G15 D11:H11" xr:uid="{26F8D555-BFDA-E840-969B-30EA98F09544}">
       <formula1>"PRESENT, ABSENT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H4 Q2:Q6 I7:I10 H11:H1048576 Q8:Q123 L10" xr:uid="{56EE3CA7-E1FA-424D-AB7B-EE80C7082F78}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H4 Q2:Q6 I7:I11 L10 Q8:Q123 H12:H1048576 C11" xr:uid="{56EE3CA7-E1FA-424D-AB7B-EE80C7082F78}">
       <formula1>$U$5:$U$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Attendance of 20-08-2023 (Sunday) and 21-08-2023 (Monday)
Attendance of 20-08-2023 (Sunday) and 21-08-2023 (Monday)
</commit_message>
<xml_diff>
--- a/React-B1-AttendanceManagement.xlsx
+++ b/React-B1-AttendanceManagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\attendanceMentainace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA553CFB-9EE1-49AC-922D-D5941BC29BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7193D8-5D0D-40DB-99E9-031A96AC30ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1637,7 +1637,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1646,7 +1646,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Office Work</t>
@@ -1661,7 +1661,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1670,7 +1670,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not responded</t>
@@ -1685,7 +1685,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1694,7 +1694,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not responded</t>
@@ -1709,7 +1709,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1718,7 +1718,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not responded</t>
@@ -1733,7 +1733,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1742,7 +1742,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Office Work</t>
@@ -1757,7 +1757,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1766,7 +1766,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not responded</t>
@@ -1781,7 +1781,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1790,7 +1790,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not responded</t>
@@ -1805,7 +1805,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1814,7 +1814,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not responded</t>
@@ -1829,7 +1829,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1838,7 +1838,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Office work</t>
@@ -1853,7 +1853,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1862,7 +1862,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Present in only first meeting not in second meeting due to office work</t>
@@ -1877,7 +1877,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1886,7 +1886,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -1901,7 +1901,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1910,7 +1910,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Medical Reason</t>
@@ -1925,7 +1925,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1934,7 +1934,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -1949,7 +1949,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1958,7 +1958,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -1973,7 +1973,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -1982,7 +1982,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Office work</t>
@@ -1997,7 +1997,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2006,7 +2006,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -2021,7 +2021,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2030,7 +2030,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -2045,7 +2045,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2054,7 +2054,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -2069,7 +2069,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2078,7 +2078,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Office work</t>
@@ -2093,7 +2093,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2102,7 +2102,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -2117,7 +2117,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2126,7 +2126,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -2141,7 +2141,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2150,7 +2150,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Outside Travelling</t>
@@ -2165,7 +2165,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2174,7 +2174,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Present in only first session absent in second session due to power failure</t>
@@ -2189,7 +2189,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2198,7 +2198,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -2213,7 +2213,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2222,7 +2222,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Office work</t>
@@ -2237,7 +2237,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2246,7 +2246,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -2261,7 +2261,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2270,7 +2270,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -2285,7 +2285,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2294,7 +2294,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -2309,7 +2309,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2318,7 +2318,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
@@ -2333,7 +2333,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Parth:</t>
         </r>
@@ -2342,10 +2342,154 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{9C002831-6667-4D3C-AFC7-AC67022251D5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Not responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{0CB57F21-5F70-4143-B694-004C723B98F0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Trevelling Outside of city</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{BD2C2E38-530A-4D4D-AFBB-8207532C43D3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Not responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K22" authorId="0" shapeId="0" xr:uid="{7B703775-BD81-445E-9FBF-1FF07EC5913E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Not responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{1EF6C138-1E41-4C78-AB62-3BDF591065B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Not responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O22" authorId="0" shapeId="0" xr:uid="{598C6F1D-AF35-4BA5-A2A3-D58A800CCB2C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Not responded</t>
         </r>
       </text>
     </comment>
@@ -2354,7 +2498,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -2435,7 +2579,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2491,19 +2635,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2977,7 +3108,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4244,42 +4375,120 @@
       <c r="A21" s="5">
         <v>45158</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
+      <c r="B21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="P21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="R21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="S21" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="T21" s="4"/>
     </row>
-    <row r="22" spans="1:20" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>45159</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="10">
+        <v>15</v>
+      </c>
+      <c r="R22" s="12">
+        <v>9</v>
+      </c>
+      <c r="S22" s="11">
+        <v>6</v>
+      </c>
       <c r="T22" s="4"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
@@ -19603,13 +19812,16 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{6155AC06-7F61-4A08-843D-AAA25B377341}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I21:P123 B5:P6 I124:K1048576 I2:P4 B2:G4 F22:G22 D23:G25 D21:G21 B26:G1048576 B8:H10 M10:P10 J8:P9 J10:K10 D11:H13 J11:P13 B11:B13 B21:B25" xr:uid="{26F8D555-BFDA-E840-969B-30EA98F09544}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11:P13 B5:P6 I124:K1048576 I2:P4 B2:G4 B11:B13 D23:G25 B23:B25 B26:G1048576 B8:H10 M10:P10 J8:P9 J10:K10 D11:H13 I23:P123" xr:uid="{26F8D555-BFDA-E840-969B-30EA98F09544}">
       <formula1>"PRESENT, ABSENT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H4 Q2:Q6 C11:C14 L10 H21:H1048576 B15:Q20 Q8:Q13 I7:I14 Q21:Q123" xr:uid="{56EE3CA7-E1FA-424D-AB7B-EE80C7082F78}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H4 Q2:Q6 C11:C14 L10 Q23:Q123 B15:Q20 Q8:Q13 I7:I14 H23:H1048576" xr:uid="{56EE3CA7-E1FA-424D-AB7B-EE80C7082F78}">
       <formula1>$U$5:$U$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21:P22" xr:uid="{2043CD1F-077B-43FF-B8AE-264E9054C4D3}">
+      <formula1>$T$5:$T$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Attendance of 26-08-2023 and 27-08-2023
Attendance of Saturday 26-08-2023 and Sunday 27-08-2023
</commit_message>
<xml_diff>
--- a/React-B1-AttendanceManagement.xlsx
+++ b/React-B1-AttendanceManagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\attendanceMentainace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CE6DCB-1108-45D9-9C27-3BFB2C70371F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2593A8C-683F-442E-8D08-087288D355D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -3092,12 +3092,108 @@
         </r>
       </text>
     </comment>
+    <comment ref="H27" authorId="0" shapeId="0" xr:uid="{7DEBF6BB-404B-4A4B-BEBD-E60859D3A2C6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Extra Study</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K27" authorId="0" shapeId="0" xr:uid="{D38D6FA0-1CF2-4549-9090-B4C17E3B4071}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L27" authorId="0" shapeId="0" xr:uid="{3D48B257-8C0C-4C08-BAEB-39A858316F57}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O27" authorId="0" shapeId="0" xr:uid="{FFE51C8C-B40E-4804-B194-AACBA25D9213}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -3684,9 +3780,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
   <dimension ref="A1:V742"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5309,17 +5405,119 @@
       <c r="A27" s="5">
         <v>45164</v>
       </c>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="10">
+        <v>15</v>
+      </c>
+      <c r="R27" s="12">
+        <v>11</v>
+      </c>
+      <c r="S27" s="11">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>45165</v>
       </c>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
+      <c r="B28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="N28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="R28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="S28" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="5">

</xml_diff>

<commit_message>
Attendance of 03-09-2023 and 04-09-2023
Attendance of 03-09-2023 (Sunday) and 04-09-2023 (Monday)
</commit_message>
<xml_diff>
--- a/React-B1-AttendanceManagement.xlsx
+++ b/React-B1-AttendanceManagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\attendanceMentainace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB45FE91-B326-49CF-9820-0FFD1B81C228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E00735-43BF-401F-BFE2-618BB7AA3858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -4076,12 +4076,156 @@
         </r>
       </text>
     </comment>
+    <comment ref="C36" authorId="0" shapeId="0" xr:uid="{0469CF07-1E5D-4293-81ED-4253BC07514F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E36" authorId="0" shapeId="0" xr:uid="{B3516E73-BE92-4407-9242-36DB39E67AAA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H36" authorId="0" shapeId="0" xr:uid="{490F23FB-C028-4C23-9385-F8C3BB80E1FE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Extra Study</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K36" authorId="0" shapeId="0" xr:uid="{A8D6E9FC-52DA-4F7D-B8DB-55ABC1904118}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L36" authorId="0" shapeId="0" xr:uid="{00E55C75-40F4-4F06-8B1A-A72BF1FB871F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O36" authorId="0" shapeId="0" xr:uid="{D76CE2E1-446A-488C-AF38-5E9B22336063}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -4675,8 +4819,8 @@
   <dimension ref="A1:V742"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6774,17 +6918,119 @@
       <c r="A35" s="5">
         <v>45172</v>
       </c>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
+      <c r="B35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="N35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="R35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="S35" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>45173</v>
       </c>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="10">
+        <v>15</v>
+      </c>
+      <c r="R36" s="12">
+        <v>9</v>
+      </c>
+      <c r="S36" s="11">
+        <v>6</v>
+      </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="5">

</xml_diff>